<commit_message>
main change: basic splitting now works. only not working yet that both parts fit together well
</commit_message>
<xml_diff>
--- a/output/inhaltsverzeichnis/csv_manual_class/manuaLclass_06_07.xlsx
+++ b/output/inhaltsverzeichnis/csv_manual_class/manuaLclass_06_07.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_1B2C379B9A254C87CB68C762B3C289D7B7435F87" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F55E57E7-6FD6-4080-B242-FAE010D54C76}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="13875"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,8 +17,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="06_07_inhaltsverzeichnis_csv" type="6" refreshedVersion="5" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="06_07_inhaltsverzeichnis_csv" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\P-Simon\Documents\SVR\output\inhaltsverzeichnis\csv\06_07_inhaltsverzeichnis_csv.txt" decimal="," thousands="." tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="194">
   <si>
     <t>```csv</t>
   </si>
@@ -562,9 +561,6 @@
     </r>
   </si>
   <si>
-    <t>Weltwirtschaft</t>
-  </si>
-  <si>
     <t xml:space="preserve">Finanzmärkte und Finanzstabilität </t>
   </si>
   <si>
@@ -660,9 +656,6 @@
     </r>
   </si>
   <si>
-    <t>LLM</t>
-  </si>
-  <si>
     <t>Kategorie Primär</t>
   </si>
   <si>
@@ -706,12 +699,18 @@
   </si>
   <si>
     <t>Europäische Union</t>
+  </si>
+  <si>
+    <t>Manuelle Klassifikation</t>
+  </si>
+  <si>
+    <t>LLM Klassifikation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -729,12 +728,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -749,14 +760,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -772,13 +788,13 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="06_07_inhaltsverzeichnis_csv" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="06_07_inhaltsverzeichnis_csv" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -816,9 +832,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -853,7 +869,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -888,7 +904,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1061,33 +1077,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H156"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="81.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1328125" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1100,14 +1119,14 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>179</v>
-      </c>
-      <c r="H2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F2" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1120,17 +1139,17 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G3" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1143,17 +1162,17 @@
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G4" t="s">
-        <v>182</v>
-      </c>
-      <c r="H4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F4" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1166,17 +1185,17 @@
       <c r="D5">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G5" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1189,17 +1208,17 @@
       <c r="D6">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G6" t="s">
-        <v>172</v>
-      </c>
-      <c r="H6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F6" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1212,17 +1231,17 @@
       <c r="D7">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G7" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1235,17 +1254,17 @@
       <c r="D8">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G8" t="s">
-        <v>183</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="F8" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G8" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1258,17 +1277,17 @@
       <c r="D9">
         <v>29</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F9" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G9" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1281,17 +1300,17 @@
       <c r="D10">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G10" t="s">
-        <v>182</v>
-      </c>
-      <c r="H10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F10" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1304,17 +1323,17 @@
       <c r="D11">
         <v>32</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G11" t="s">
-        <v>182</v>
-      </c>
-      <c r="H11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F11" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1327,17 +1346,17 @@
       <c r="D12">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G12" t="s">
+      <c r="F12" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="H12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1350,17 +1369,17 @@
       <c r="D13">
         <v>40</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G13" t="s">
-        <v>182</v>
-      </c>
-      <c r="H13" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F13" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1373,17 +1392,17 @@
       <c r="D14">
         <v>42</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G14" t="s">
-        <v>182</v>
-      </c>
-      <c r="H14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F14" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1396,17 +1415,17 @@
       <c r="D15">
         <v>43</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G15" t="s">
-        <v>182</v>
-      </c>
-      <c r="H15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F15" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1419,17 +1438,17 @@
       <c r="D16">
         <v>45</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G16" t="s">
-        <v>182</v>
-      </c>
-      <c r="H16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F16" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1442,17 +1461,17 @@
       <c r="D17">
         <v>48</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G17" t="s">
-        <v>182</v>
-      </c>
-      <c r="H17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F17" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1465,17 +1484,17 @@
       <c r="D18">
         <v>50</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G18" t="s">
-        <v>182</v>
-      </c>
-      <c r="H18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F18" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1488,17 +1507,17 @@
       <c r="D19">
         <v>51</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G19" t="s">
-        <v>182</v>
-      </c>
-      <c r="H19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F19" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1511,17 +1530,17 @@
       <c r="D20">
         <v>56</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G20" t="s">
-        <v>182</v>
-      </c>
-      <c r="H20" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F20" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1534,17 +1553,17 @@
       <c r="D21">
         <v>64</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G21" t="s">
-        <v>182</v>
-      </c>
-      <c r="H21" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F21" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1557,17 +1576,17 @@
       <c r="D22">
         <v>64</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G22" t="s">
-        <v>182</v>
-      </c>
-      <c r="H22" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F22" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1580,17 +1599,17 @@
       <c r="D23">
         <v>70</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G23" t="s">
-        <v>182</v>
-      </c>
-      <c r="H23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F23" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1603,17 +1622,17 @@
       <c r="D24">
         <v>71</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G24" t="s">
-        <v>188</v>
-      </c>
-      <c r="H24" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F24" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1626,17 +1645,17 @@
       <c r="D25">
         <v>73</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G25" t="s">
-        <v>182</v>
-      </c>
-      <c r="H25" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F25" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1649,17 +1668,17 @@
       <c r="D26">
         <v>77</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G26" t="s">
-        <v>182</v>
-      </c>
-      <c r="H26" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F26" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1672,17 +1691,17 @@
       <c r="D27">
         <v>79</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G27" t="s">
-        <v>182</v>
-      </c>
-      <c r="H27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F27" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1695,17 +1714,17 @@
       <c r="D28">
         <v>82</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G28" t="s">
-        <v>182</v>
-      </c>
-      <c r="H28" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F28" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1718,17 +1737,17 @@
       <c r="D29">
         <v>86</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G29" t="s">
-        <v>182</v>
-      </c>
-      <c r="H29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F29" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1741,17 +1760,17 @@
       <c r="D30">
         <v>86</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G30" t="s">
-        <v>182</v>
-      </c>
-      <c r="H30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F30" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1764,17 +1783,17 @@
       <c r="D31">
         <v>91</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G31" t="s">
-        <v>182</v>
-      </c>
-      <c r="H31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F31" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1787,17 +1806,17 @@
       <c r="D32">
         <v>103</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G32" t="s">
-        <v>189</v>
-      </c>
-      <c r="H32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F32" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1810,17 +1829,17 @@
       <c r="D33">
         <v>108</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G33" t="s">
+      <c r="F33" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G33" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1833,20 +1852,17 @@
       <c r="D34">
         <v>110</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F34" t="s">
-        <v>166</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F34" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G34" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1859,17 +1875,17 @@
       <c r="D35">
         <v>112</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G35" t="s">
+      <c r="F35" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H35" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G35" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1882,20 +1898,17 @@
       <c r="D36">
         <v>112</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F36" t="s">
-        <v>167</v>
-      </c>
-      <c r="G36" t="s">
-        <v>188</v>
-      </c>
-      <c r="H36" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F36" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1908,20 +1921,17 @@
       <c r="D37">
         <v>118</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F37" t="s">
-        <v>167</v>
-      </c>
-      <c r="G37" t="s">
-        <v>190</v>
-      </c>
-      <c r="H37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F37" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1934,20 +1944,17 @@
       <c r="D38">
         <v>120</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F38" t="s">
-        <v>167</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="F38" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G38" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1960,20 +1967,17 @@
       <c r="D39">
         <v>122</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F39" t="s">
-        <v>167</v>
-      </c>
-      <c r="G39" t="s">
-        <v>188</v>
-      </c>
-      <c r="H39" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F39" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1986,20 +1990,17 @@
       <c r="D40">
         <v>122</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F40" t="s">
-        <v>167</v>
-      </c>
-      <c r="G40" t="s">
-        <v>188</v>
-      </c>
-      <c r="H40" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F40" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -2012,20 +2013,17 @@
       <c r="D41">
         <v>125</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F41" t="s">
-        <v>167</v>
-      </c>
-      <c r="G41" t="s">
-        <v>188</v>
-      </c>
-      <c r="H41" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F41" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2038,20 +2036,17 @@
       <c r="D42">
         <v>128</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F42" t="s">
-        <v>167</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="F42" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G42" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2064,20 +2059,17 @@
       <c r="D43">
         <v>129</v>
       </c>
-      <c r="E43" t="s">
-        <v>168</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="E43" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G43" t="s">
-        <v>190</v>
-      </c>
-      <c r="H43" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F43" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -2090,20 +2082,17 @@
       <c r="D44">
         <v>130</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F44" t="s">
-        <v>167</v>
-      </c>
-      <c r="G44" t="s">
-        <v>188</v>
-      </c>
-      <c r="H44" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F44" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -2116,20 +2105,17 @@
       <c r="D45">
         <v>133</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F45" t="s">
-        <v>167</v>
-      </c>
-      <c r="G45" t="s">
-        <v>188</v>
-      </c>
-      <c r="H45" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F45" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -2142,20 +2128,17 @@
       <c r="D46">
         <v>136</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F46" t="s">
-        <v>167</v>
-      </c>
-      <c r="G46" t="s">
-        <v>182</v>
-      </c>
-      <c r="H46" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F46" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -2168,20 +2151,17 @@
       <c r="D47">
         <v>137</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F47" t="s">
-        <v>167</v>
-      </c>
-      <c r="G47" t="s">
-        <v>182</v>
-      </c>
-      <c r="H47" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F47" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -2194,20 +2174,17 @@
       <c r="D48">
         <v>139</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F48" t="s">
-        <v>167</v>
-      </c>
-      <c r="G48" t="s">
+      <c r="F48" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H48" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G48" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -2220,20 +2197,17 @@
       <c r="D49">
         <v>139</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F49" t="s">
-        <v>167</v>
-      </c>
-      <c r="G49" t="s">
+      <c r="F49" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G49" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -2246,20 +2220,17 @@
       <c r="D50">
         <v>143</v>
       </c>
-      <c r="E50" t="s">
-        <v>168</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E50" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G50" t="s">
-        <v>168</v>
-      </c>
-      <c r="H50" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F50" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -2272,17 +2243,17 @@
       <c r="D51">
         <v>145</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G51" t="s">
+      <c r="F51" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H51" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G51" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -2295,17 +2266,17 @@
       <c r="D52">
         <v>145</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G52" t="s">
-        <v>189</v>
-      </c>
-      <c r="H52" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F52" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -2318,14 +2289,14 @@
       <c r="D53">
         <v>146</v>
       </c>
-      <c r="G53" t="s">
-        <v>189</v>
-      </c>
-      <c r="H53" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F53" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -2338,17 +2309,17 @@
       <c r="D54">
         <v>146</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G54" t="s">
-        <v>188</v>
-      </c>
-      <c r="H54" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F54" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -2361,17 +2332,17 @@
       <c r="D55">
         <v>149</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G55" t="s">
-        <v>188</v>
-      </c>
-      <c r="H55" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F55" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -2384,17 +2355,17 @@
       <c r="D56">
         <v>150</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G56" t="s">
+      <c r="F56" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H56" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G56" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -2407,17 +2378,17 @@
       <c r="D57">
         <v>154</v>
       </c>
-      <c r="E57" t="s">
-        <v>170</v>
-      </c>
-      <c r="G57" t="s">
-        <v>190</v>
-      </c>
-      <c r="H57" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E57" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -2430,17 +2401,17 @@
       <c r="D58">
         <v>156</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G58" t="s">
+      <c r="F58" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H58" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G58" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>36</v>
       </c>
@@ -2453,17 +2424,17 @@
       <c r="D59">
         <v>157</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G59" t="s">
-        <v>182</v>
-      </c>
-      <c r="H59" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F59" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>36</v>
       </c>
@@ -2476,17 +2447,17 @@
       <c r="D60">
         <v>158</v>
       </c>
-      <c r="E60" t="s">
-        <v>170</v>
-      </c>
-      <c r="G60" t="s">
-        <v>190</v>
-      </c>
-      <c r="H60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E60" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -2499,17 +2470,17 @@
       <c r="D61">
         <v>159</v>
       </c>
-      <c r="E61" t="s">
-        <v>169</v>
-      </c>
-      <c r="G61" t="s">
-        <v>169</v>
-      </c>
-      <c r="H61" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E61" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -2522,17 +2493,17 @@
       <c r="D62">
         <v>164</v>
       </c>
-      <c r="E62" t="s">
-        <v>170</v>
-      </c>
-      <c r="G62" t="s">
+      <c r="E62" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H62" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G62" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -2545,17 +2516,17 @@
       <c r="D63">
         <v>166</v>
       </c>
-      <c r="E63" t="s">
-        <v>170</v>
-      </c>
-      <c r="G63" t="s">
-        <v>190</v>
-      </c>
-      <c r="H63" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E63" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -2568,17 +2539,17 @@
       <c r="D64">
         <v>167</v>
       </c>
-      <c r="E64" t="s">
-        <v>170</v>
-      </c>
-      <c r="G64" t="s">
-        <v>190</v>
-      </c>
-      <c r="H64" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E64" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2591,17 +2562,17 @@
       <c r="D65">
         <v>172</v>
       </c>
-      <c r="E65" t="s">
-        <v>170</v>
-      </c>
-      <c r="G65" t="s">
-        <v>190</v>
-      </c>
-      <c r="H65" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E65" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2614,17 +2585,17 @@
       <c r="D66">
         <v>174</v>
       </c>
-      <c r="E66" t="s">
-        <v>170</v>
-      </c>
-      <c r="G66" t="s">
-        <v>190</v>
-      </c>
-      <c r="H66" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E66" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -2637,17 +2608,17 @@
       <c r="D67">
         <v>181</v>
       </c>
-      <c r="E67" t="s">
-        <v>170</v>
-      </c>
-      <c r="G67" t="s">
-        <v>168</v>
-      </c>
-      <c r="H67" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E67" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -2660,17 +2631,17 @@
       <c r="D68">
         <v>183</v>
       </c>
-      <c r="E68" t="s">
-        <v>170</v>
-      </c>
-      <c r="G68" t="s">
-        <v>168</v>
-      </c>
-      <c r="H68" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E68" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>65</v>
       </c>
@@ -2683,17 +2654,17 @@
       <c r="D69">
         <v>185</v>
       </c>
-      <c r="E69" t="s">
-        <v>170</v>
-      </c>
-      <c r="G69" t="s">
-        <v>190</v>
-      </c>
-      <c r="H69" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E69" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>65</v>
       </c>
@@ -2706,17 +2677,17 @@
       <c r="D70">
         <v>187</v>
       </c>
-      <c r="E70" t="s">
-        <v>170</v>
-      </c>
-      <c r="G70" t="s">
-        <v>190</v>
-      </c>
-      <c r="H70" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E70" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>65</v>
       </c>
@@ -2729,17 +2700,17 @@
       <c r="D71">
         <v>189</v>
       </c>
-      <c r="E71" t="s">
-        <v>170</v>
-      </c>
-      <c r="G71" t="s">
-        <v>190</v>
-      </c>
-      <c r="H71" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E71" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>65</v>
       </c>
@@ -2752,17 +2723,17 @@
       <c r="D72">
         <v>191</v>
       </c>
-      <c r="E72" t="s">
-        <v>170</v>
-      </c>
-      <c r="G72" t="s">
-        <v>190</v>
-      </c>
-      <c r="H72" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E72" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>65</v>
       </c>
@@ -2775,17 +2746,17 @@
       <c r="D73">
         <v>192</v>
       </c>
-      <c r="E73" t="s">
-        <v>170</v>
-      </c>
-      <c r="G73" t="s">
-        <v>190</v>
-      </c>
-      <c r="H73" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E73" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>65</v>
       </c>
@@ -2798,17 +2769,17 @@
       <c r="D74">
         <v>194</v>
       </c>
-      <c r="E74" t="s">
-        <v>170</v>
-      </c>
-      <c r="G74" t="s">
-        <v>190</v>
-      </c>
-      <c r="H74" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E74" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>65</v>
       </c>
@@ -2821,17 +2792,17 @@
       <c r="D75">
         <v>196</v>
       </c>
-      <c r="E75" t="s">
-        <v>170</v>
-      </c>
-      <c r="G75" t="s">
-        <v>190</v>
-      </c>
-      <c r="H75" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E75" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>65</v>
       </c>
@@ -2844,17 +2815,17 @@
       <c r="D76">
         <v>198</v>
       </c>
-      <c r="E76" t="s">
-        <v>170</v>
-      </c>
-      <c r="G76" t="s">
-        <v>190</v>
-      </c>
-      <c r="H76" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E76" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>65</v>
       </c>
@@ -2867,17 +2838,17 @@
       <c r="D77">
         <v>199</v>
       </c>
-      <c r="E77" t="s">
-        <v>170</v>
-      </c>
-      <c r="G77" t="s">
-        <v>168</v>
-      </c>
-      <c r="H77" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E77" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>65</v>
       </c>
@@ -2890,17 +2861,17 @@
       <c r="D78">
         <v>200</v>
       </c>
-      <c r="E78" t="s">
-        <v>170</v>
-      </c>
-      <c r="G78" t="s">
-        <v>168</v>
-      </c>
-      <c r="H78" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E78" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>65</v>
       </c>
@@ -2913,17 +2884,17 @@
       <c r="D79">
         <v>204</v>
       </c>
-      <c r="E79" t="s">
-        <v>170</v>
-      </c>
-      <c r="G79" t="s">
-        <v>168</v>
-      </c>
-      <c r="H79" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E79" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>65</v>
       </c>
@@ -2936,17 +2907,17 @@
       <c r="D80">
         <v>205</v>
       </c>
-      <c r="E80" t="s">
-        <v>170</v>
-      </c>
-      <c r="G80" t="s">
-        <v>168</v>
-      </c>
-      <c r="H80" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E80" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>65</v>
       </c>
@@ -2959,17 +2930,17 @@
       <c r="D81">
         <v>206</v>
       </c>
-      <c r="E81" t="s">
-        <v>170</v>
-      </c>
-      <c r="G81" t="s">
-        <v>168</v>
-      </c>
-      <c r="H81" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E81" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -2982,17 +2953,17 @@
       <c r="D82">
         <v>210</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G82" t="s">
+      <c r="E82" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F82" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H82" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G82" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>85</v>
       </c>
@@ -3005,17 +2976,17 @@
       <c r="D83">
         <v>213</v>
       </c>
-      <c r="E83" t="s">
-        <v>171</v>
-      </c>
-      <c r="G83" t="s">
-        <v>174</v>
-      </c>
-      <c r="H83" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E83" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>85</v>
       </c>
@@ -3028,17 +2999,17 @@
       <c r="D84">
         <v>213</v>
       </c>
-      <c r="E84" t="s">
-        <v>171</v>
-      </c>
-      <c r="G84" t="s">
-        <v>174</v>
-      </c>
-      <c r="H84" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E84" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -3051,17 +3022,17 @@
       <c r="D85">
         <v>216</v>
       </c>
-      <c r="E85" t="s">
-        <v>171</v>
-      </c>
-      <c r="G85" t="s">
-        <v>174</v>
-      </c>
-      <c r="H85" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E85" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -3074,17 +3045,17 @@
       <c r="D86">
         <v>217</v>
       </c>
-      <c r="E86" t="s">
-        <v>171</v>
-      </c>
-      <c r="G86" t="s">
-        <v>174</v>
-      </c>
-      <c r="H86" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -3097,17 +3068,17 @@
       <c r="D87">
         <v>217</v>
       </c>
-      <c r="E87" t="s">
-        <v>171</v>
-      </c>
-      <c r="G87" t="s">
-        <v>174</v>
-      </c>
-      <c r="H87" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E87" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -3120,17 +3091,17 @@
       <c r="D88">
         <v>219</v>
       </c>
-      <c r="E88" t="s">
-        <v>171</v>
-      </c>
-      <c r="G88" t="s">
-        <v>174</v>
-      </c>
-      <c r="H88" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E88" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -3143,17 +3114,17 @@
       <c r="D89">
         <v>223</v>
       </c>
-      <c r="E89" t="s">
-        <v>171</v>
-      </c>
-      <c r="G89" t="s">
-        <v>174</v>
-      </c>
-      <c r="H89" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E89" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -3166,17 +3137,17 @@
       <c r="D90">
         <v>226</v>
       </c>
-      <c r="E90" t="s">
-        <v>171</v>
-      </c>
-      <c r="G90" t="s">
-        <v>174</v>
-      </c>
-      <c r="H90" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E90" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -3189,17 +3160,17 @@
       <c r="D91">
         <v>228</v>
       </c>
-      <c r="E91" t="s">
-        <v>171</v>
-      </c>
-      <c r="G91" t="s">
-        <v>176</v>
-      </c>
-      <c r="H91" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E91" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>85</v>
       </c>
@@ -3212,17 +3183,17 @@
       <c r="D92">
         <v>230</v>
       </c>
-      <c r="E92" t="s">
-        <v>171</v>
-      </c>
-      <c r="G92" t="s">
-        <v>174</v>
-      </c>
-      <c r="H92" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E92" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>85</v>
       </c>
@@ -3235,17 +3206,17 @@
       <c r="D93">
         <v>230</v>
       </c>
-      <c r="E93" t="s">
-        <v>171</v>
-      </c>
-      <c r="G93" t="s">
-        <v>174</v>
-      </c>
-      <c r="H93" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E93" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>85</v>
       </c>
@@ -3258,17 +3229,17 @@
       <c r="D94">
         <v>230</v>
       </c>
-      <c r="E94" t="s">
-        <v>171</v>
-      </c>
-      <c r="G94" t="s">
-        <v>174</v>
-      </c>
-      <c r="H94" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E94" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>85</v>
       </c>
@@ -3281,17 +3252,17 @@
       <c r="D95">
         <v>231</v>
       </c>
-      <c r="E95" t="s">
-        <v>171</v>
-      </c>
-      <c r="G95" t="s">
-        <v>174</v>
-      </c>
-      <c r="H95" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E95" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>85</v>
       </c>
@@ -3304,17 +3275,17 @@
       <c r="D96">
         <v>232</v>
       </c>
-      <c r="E96" t="s">
-        <v>171</v>
-      </c>
-      <c r="G96" t="s">
-        <v>174</v>
-      </c>
-      <c r="H96" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E96" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>85</v>
       </c>
@@ -3327,17 +3298,17 @@
       <c r="D97">
         <v>233</v>
       </c>
-      <c r="E97" t="s">
-        <v>171</v>
-      </c>
-      <c r="G97" t="s">
-        <v>174</v>
-      </c>
-      <c r="H97" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E97" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>85</v>
       </c>
@@ -3350,17 +3321,17 @@
       <c r="D98">
         <v>233</v>
       </c>
-      <c r="E98" t="s">
-        <v>171</v>
-      </c>
-      <c r="G98" t="s">
-        <v>174</v>
-      </c>
-      <c r="H98" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E98" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>85</v>
       </c>
@@ -3373,17 +3344,17 @@
       <c r="D99">
         <v>234</v>
       </c>
-      <c r="E99" t="s">
-        <v>171</v>
-      </c>
-      <c r="G99" t="s">
-        <v>174</v>
-      </c>
-      <c r="H99" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E99" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>85</v>
       </c>
@@ -3396,17 +3367,17 @@
       <c r="D100">
         <v>236</v>
       </c>
-      <c r="E100" t="s">
-        <v>174</v>
-      </c>
-      <c r="G100" t="s">
-        <v>174</v>
-      </c>
-      <c r="H100" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E100" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>85</v>
       </c>
@@ -3419,17 +3390,17 @@
       <c r="D101">
         <v>236</v>
       </c>
-      <c r="E101" t="s">
-        <v>173</v>
-      </c>
-      <c r="G101" t="s">
-        <v>191</v>
-      </c>
-      <c r="H101" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E101" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>85</v>
       </c>
@@ -3442,17 +3413,17 @@
       <c r="D102">
         <v>237</v>
       </c>
-      <c r="E102" t="s">
-        <v>173</v>
-      </c>
-      <c r="G102" t="s">
-        <v>191</v>
-      </c>
-      <c r="H102" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E102" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>85</v>
       </c>
@@ -3465,17 +3436,17 @@
       <c r="D103">
         <v>237</v>
       </c>
-      <c r="E103" t="s">
-        <v>173</v>
-      </c>
-      <c r="G103" t="s">
-        <v>191</v>
-      </c>
-      <c r="H103" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E103" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>85</v>
       </c>
@@ -3488,17 +3459,17 @@
       <c r="D104">
         <v>238</v>
       </c>
-      <c r="E104" t="s">
-        <v>173</v>
-      </c>
-      <c r="G104" t="s">
-        <v>191</v>
-      </c>
-      <c r="H104" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E104" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>85</v>
       </c>
@@ -3511,17 +3482,17 @@
       <c r="D105">
         <v>241</v>
       </c>
-      <c r="E105" t="s">
-        <v>173</v>
-      </c>
-      <c r="G105" t="s">
-        <v>191</v>
-      </c>
-      <c r="H105" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E105" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>85</v>
       </c>
@@ -3534,17 +3505,17 @@
       <c r="D106">
         <v>253</v>
       </c>
-      <c r="E106" t="s">
-        <v>173</v>
-      </c>
-      <c r="G106" t="s">
-        <v>191</v>
-      </c>
-      <c r="H106" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E106" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>85</v>
       </c>
@@ -3557,17 +3528,17 @@
       <c r="D107">
         <v>254</v>
       </c>
-      <c r="E107" t="s">
-        <v>173</v>
-      </c>
-      <c r="G107" t="s">
-        <v>191</v>
-      </c>
-      <c r="H107" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E107" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>85</v>
       </c>
@@ -3580,17 +3551,17 @@
       <c r="D108">
         <v>255</v>
       </c>
-      <c r="E108" t="s">
-        <v>173</v>
-      </c>
-      <c r="G108" t="s">
-        <v>191</v>
-      </c>
-      <c r="H108" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E108" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>85</v>
       </c>
@@ -3603,17 +3574,17 @@
       <c r="D109">
         <v>258</v>
       </c>
-      <c r="E109" t="s">
-        <v>173</v>
-      </c>
-      <c r="G109" t="s">
-        <v>191</v>
-      </c>
-      <c r="H109" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E109" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G109" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>85</v>
       </c>
@@ -3626,17 +3597,17 @@
       <c r="D110">
         <v>258</v>
       </c>
-      <c r="E110" t="s">
-        <v>173</v>
-      </c>
-      <c r="G110" t="s">
-        <v>191</v>
-      </c>
-      <c r="H110" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E110" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>85</v>
       </c>
@@ -3649,17 +3620,17 @@
       <c r="D111">
         <v>258</v>
       </c>
-      <c r="E111" t="s">
-        <v>173</v>
-      </c>
-      <c r="G111" t="s">
-        <v>191</v>
-      </c>
-      <c r="H111" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E111" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G111" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>85</v>
       </c>
@@ -3672,17 +3643,17 @@
       <c r="D112">
         <v>260</v>
       </c>
-      <c r="E112" t="s">
-        <v>173</v>
-      </c>
-      <c r="G112" t="s">
-        <v>191</v>
-      </c>
-      <c r="H112" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E112" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>85</v>
       </c>
@@ -3695,17 +3666,17 @@
       <c r="D113">
         <v>260</v>
       </c>
-      <c r="E113" t="s">
-        <v>173</v>
-      </c>
-      <c r="G113" t="s">
-        <v>191</v>
-      </c>
-      <c r="H113" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E113" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G113" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>85</v>
       </c>
@@ -3718,17 +3689,17 @@
       <c r="D114">
         <v>261</v>
       </c>
-      <c r="E114" t="s">
-        <v>173</v>
-      </c>
-      <c r="G114" t="s">
-        <v>191</v>
-      </c>
-      <c r="H114" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E114" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>85</v>
       </c>
@@ -3741,17 +3712,17 @@
       <c r="D115">
         <v>262</v>
       </c>
-      <c r="E115" t="s">
-        <v>173</v>
-      </c>
-      <c r="G115" t="s">
-        <v>191</v>
-      </c>
-      <c r="H115" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E115" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G115" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>85</v>
       </c>
@@ -3764,17 +3735,17 @@
       <c r="D116">
         <v>262</v>
       </c>
-      <c r="E116" t="s">
-        <v>173</v>
-      </c>
-      <c r="G116" t="s">
-        <v>191</v>
-      </c>
-      <c r="H116" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E116" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G116" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>85</v>
       </c>
@@ -3787,17 +3758,17 @@
       <c r="D117">
         <v>263</v>
       </c>
-      <c r="E117" t="s">
-        <v>173</v>
-      </c>
-      <c r="G117" t="s">
-        <v>191</v>
-      </c>
-      <c r="H117" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E117" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G117" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>85</v>
       </c>
@@ -3810,17 +3781,17 @@
       <c r="D118">
         <v>268</v>
       </c>
-      <c r="E118" t="s">
-        <v>173</v>
-      </c>
-      <c r="G118" t="s">
-        <v>191</v>
-      </c>
-      <c r="H118" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E118" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G118" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>85</v>
       </c>
@@ -3833,17 +3804,17 @@
       <c r="D119">
         <v>275</v>
       </c>
-      <c r="E119" t="s">
-        <v>174</v>
-      </c>
-      <c r="G119" t="s">
-        <v>174</v>
-      </c>
-      <c r="H119" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E119" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G119" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>85</v>
       </c>
@@ -3856,17 +3827,17 @@
       <c r="D120">
         <v>275</v>
       </c>
-      <c r="E120" t="s">
-        <v>175</v>
-      </c>
-      <c r="G120" t="s">
-        <v>192</v>
-      </c>
-      <c r="H120" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E120" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="G120" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>124</v>
       </c>
@@ -3879,17 +3850,17 @@
       <c r="D121">
         <v>280</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E121" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G121" t="s">
+      <c r="F121" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H121" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G121" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>124</v>
       </c>
@@ -3902,17 +3873,17 @@
       <c r="D122">
         <v>282</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G122" t="s">
-        <v>189</v>
-      </c>
-      <c r="H122" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F122" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G122" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>124</v>
       </c>
@@ -3925,17 +3896,17 @@
       <c r="D123">
         <v>282</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G123" t="s">
-        <v>189</v>
-      </c>
-      <c r="H123" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F123" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G123" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>124</v>
       </c>
@@ -3948,17 +3919,17 @@
       <c r="D124">
         <v>287</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G124" t="s">
-        <v>189</v>
-      </c>
-      <c r="H124" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F124" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -3971,17 +3942,17 @@
       <c r="D125">
         <v>288</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E125" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G125" t="s">
-        <v>176</v>
-      </c>
-      <c r="H125" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F125" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G125" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -3994,17 +3965,17 @@
       <c r="D126">
         <v>293</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G126" t="s">
-        <v>189</v>
-      </c>
-      <c r="H126" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F126" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G126" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>124</v>
       </c>
@@ -4017,17 +3988,17 @@
       <c r="D127">
         <v>296</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E127" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G127" t="s">
-        <v>189</v>
-      </c>
-      <c r="H127" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F127" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G127" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>124</v>
       </c>
@@ -4040,17 +4011,17 @@
       <c r="D128">
         <v>299</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E128" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G128" t="s">
-        <v>189</v>
-      </c>
-      <c r="H128" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F128" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G128" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>124</v>
       </c>
@@ -4063,17 +4034,17 @@
       <c r="D129">
         <v>299</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E129" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G129" t="s">
-        <v>193</v>
-      </c>
-      <c r="H129" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F129" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G129" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>124</v>
       </c>
@@ -4086,17 +4057,17 @@
       <c r="D130">
         <v>300</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E130" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G130" t="s">
-        <v>189</v>
-      </c>
-      <c r="H130" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F130" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>124</v>
       </c>
@@ -4109,17 +4080,17 @@
       <c r="D131">
         <v>308</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E131" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G131" t="s">
-        <v>189</v>
-      </c>
-      <c r="H131" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F131" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>124</v>
       </c>
@@ -4132,11 +4103,11 @@
       <c r="D132">
         <v>311</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E132" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>124</v>
       </c>
@@ -4149,11 +4120,11 @@
       <c r="D133">
         <v>316</v>
       </c>
-      <c r="E133" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E133" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>124</v>
       </c>
@@ -4166,11 +4137,11 @@
       <c r="D134">
         <v>317</v>
       </c>
-      <c r="E134" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E134" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>124</v>
       </c>
@@ -4183,11 +4154,11 @@
       <c r="D135">
         <v>321</v>
       </c>
-      <c r="E135" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E135" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>124</v>
       </c>
@@ -4200,11 +4171,11 @@
       <c r="D136">
         <v>323</v>
       </c>
-      <c r="E136" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E136" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>124</v>
       </c>
@@ -4217,11 +4188,11 @@
       <c r="D137">
         <v>326</v>
       </c>
-      <c r="E137" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E137" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>124</v>
       </c>
@@ -4234,11 +4205,11 @@
       <c r="D138">
         <v>336</v>
       </c>
-      <c r="E138" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E138" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>124</v>
       </c>
@@ -4251,11 +4222,11 @@
       <c r="D139">
         <v>338</v>
       </c>
-      <c r="E139" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E139" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>124</v>
       </c>
@@ -4268,11 +4239,11 @@
       <c r="D140">
         <v>339</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>124</v>
       </c>
@@ -4285,11 +4256,11 @@
       <c r="D141">
         <v>344</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E141" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>145</v>
       </c>
@@ -4302,11 +4273,11 @@
       <c r="D142">
         <v>352</v>
       </c>
-      <c r="E142" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E142" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>145</v>
       </c>
@@ -4319,11 +4290,11 @@
       <c r="D143">
         <v>354</v>
       </c>
-      <c r="E143" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E143" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>145</v>
       </c>
@@ -4336,11 +4307,11 @@
       <c r="D144">
         <v>354</v>
       </c>
-      <c r="E144" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E144" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>145</v>
       </c>
@@ -4353,11 +4324,11 @@
       <c r="D145">
         <v>359</v>
       </c>
-      <c r="E145" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E145" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -4370,11 +4341,11 @@
       <c r="D146">
         <v>362</v>
       </c>
-      <c r="E146" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E146" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -4387,11 +4358,11 @@
       <c r="D147">
         <v>362</v>
       </c>
-      <c r="E147" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E147" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>145</v>
       </c>
@@ -4404,11 +4375,11 @@
       <c r="D148">
         <v>365</v>
       </c>
-      <c r="E148" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E148" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>145</v>
       </c>
@@ -4421,11 +4392,11 @@
       <c r="D149">
         <v>371</v>
       </c>
-      <c r="E149" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E149" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>145</v>
       </c>
@@ -4438,11 +4409,11 @@
       <c r="D150">
         <v>371</v>
       </c>
-      <c r="E150" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E150" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>145</v>
       </c>
@@ -4455,11 +4426,11 @@
       <c r="D151">
         <v>372</v>
       </c>
-      <c r="E151" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E151" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>145</v>
       </c>
@@ -4472,11 +4443,11 @@
       <c r="D152">
         <v>373</v>
       </c>
-      <c r="E152" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E152" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>145</v>
       </c>
@@ -4489,11 +4460,11 @@
       <c r="D153">
         <v>374</v>
       </c>
-      <c r="E153" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E153" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>145</v>
       </c>
@@ -4506,11 +4477,11 @@
       <c r="D154">
         <v>375</v>
       </c>
-      <c r="E154" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E154" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>145</v>
       </c>
@@ -4523,19 +4494,22 @@
       <c r="D155">
         <v>376</v>
       </c>
-      <c r="E155" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E155" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>159</v>
       </c>
-      <c r="E156" t="s">
-        <v>177</v>
+      <c r="E156" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>